<commit_message>
Fixes bulk upload tests
</commit_message>
<xml_diff>
--- a/DigitalLearningSolutions.Web.Tests/TestData/DelegateUploadTest.xlsx
+++ b/DigitalLearningSolutions.Web.Tests/TestData/DelegateUploadTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejac\Git\DLSV2\DigitalLearningSolutions.Data.Tests\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\digitallearningsolutions\DigitalLearningSolutions.Web.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9638E091-4EC5-40B1-A2AD-7AD694CC5E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E547F8FC-808F-4D88-ABAF-40076778F482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28898" yWindow="6278" windowWidth="28996" windowHeight="15795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DelegatesBulkUpload" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>LastName</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>MammalHands</t>
+  </si>
+  <si>
+    <t>JobGroup</t>
   </si>
 </sst>
 </file>
@@ -159,10 +162,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -182,13 +184,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:N4" totalsRowShown="0">
-  <autoFilter ref="A1:N4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O4" totalsRowShown="0">
+  <autoFilter ref="A1:O4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DelegateID"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="LastName"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="FirstName"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="DelegateID"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="JobGroupID"/>
+    <tableColumn id="4" xr3:uid="{9D8751C0-3D1F-42DD-A958-9EAEB079D219}" name="JobGroup"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Answer1"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Answer2"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Answer3"/>
@@ -500,152 +503,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
-    <col min="12" max="12" width="24.42578125" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" customWidth="1"/>
+    <col min="5" max="6" width="14.54296875" customWidth="1"/>
+    <col min="7" max="7" width="47.81640625" customWidth="1"/>
+    <col min="8" max="8" width="28.1796875" customWidth="1"/>
+    <col min="9" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="9.81640625" customWidth="1"/>
+    <col min="14" max="14" width="24.453125" customWidth="1"/>
+    <col min="15" max="15" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="K2" t="b">
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="b">
         <v>1</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="2" t="b">
+      <c r="N2" t="b">
         <v>0</v>
       </c>
-      <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="K3" t="b">
+      <c r="L3" t="b">
         <v>1</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" t="b">
+      <c r="L4" t="b">
         <v>1</v>
       </c>
-      <c r="M4" s="2" t="b">
+      <c r="N4" t="b">
         <v>1</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{834F36E7-56E3-4E88-B49C-CF3ABF387582}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{834F36E7-56E3-4E88-B49C-CF3ABF387582}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <tableParts count="1">
@@ -658,17 +668,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -676,28 +684,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>